<commit_message>
reknit IHC with all data
</commit_message>
<xml_diff>
--- a/data/IHC/coloc2-pgp-totals.xlsx
+++ b/data/IHC/coloc2-pgp-totals.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve">sex</t>
   </si>
@@ -50,18 +50,54 @@
     <t xml:space="preserve">F</t>
   </si>
   <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slide1-section2-20x-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slide1-section2-20x-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slide1-section3-20x-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slide1-section3-20x-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slide2-section2-20x-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slide2-section2-20x-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GFP-wm-20x-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GFP-wm-20x-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GFP-wm-20x-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GFP-wm2-20x-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">87</t>
   </si>
   <si>
-    <t xml:space="preserve">wm</t>
-  </si>
-  <si>
     <t xml:space="preserve">wm-20x-1</t>
   </si>
   <si>
-    <t xml:space="preserve">TRUE</t>
-  </si>
-  <si>
     <t xml:space="preserve">wm-20x-2</t>
   </si>
   <si>
@@ -80,15 +116,6 @@
     <t xml:space="preserve">10</t>
   </si>
   <si>
-    <t xml:space="preserve">GFP-wm-20x-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GFP-wm-20x-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GFP-wm-20x-3</t>
-  </si>
-  <si>
     <t xml:space="preserve">GFP-wm-20x-4</t>
   </si>
   <si>
@@ -99,9 +126,6 @@
   </si>
   <si>
     <t xml:space="preserve">80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">section</t>
   </si>
   <si>
     <t xml:space="preserve">section1-1</t>
@@ -512,25 +536,25 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01</v>
+        <v>0.816</v>
       </c>
       <c r="F2" t="n">
-        <v>0.047</v>
+        <v>0.76</v>
       </c>
       <c r="G2" t="n">
-        <v>0.21</v>
+        <v>0.64</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
-        <v>15</v>
+      <c r="K2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -544,28 +568,28 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" t="n">
-        <v>0.021</v>
+        <v>0.789</v>
       </c>
       <c r="F3" t="n">
-        <v>0.044</v>
+        <v>0.77</v>
       </c>
       <c r="G3" t="n">
-        <v>0.28</v>
+        <v>0.58</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
-      <c r="K3" t="s">
-        <v>15</v>
+      <c r="K3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -579,16 +603,16 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" t="n">
-        <v>0.655</v>
+        <v>0.845</v>
       </c>
       <c r="F4" t="n">
-        <v>0.585</v>
+        <v>0.64</v>
       </c>
       <c r="G4" t="n">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -599,8 +623,8 @@
       <c r="J4" t="n">
         <v>0</v>
       </c>
-      <c r="K4" t="s">
-        <v>15</v>
+      <c r="K4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -614,28 +638,28 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" t="n">
-        <v>0.719</v>
+        <v>0.063</v>
       </c>
       <c r="F5" t="n">
-        <v>0.479</v>
+        <v>0.057</v>
       </c>
       <c r="G5" t="n">
-        <v>0.38</v>
+        <v>0.61</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
       </c>
-      <c r="K5" t="s">
-        <v>15</v>
+      <c r="K5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -649,16 +673,16 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="n">
-        <v>0.674</v>
+        <v>0.613</v>
       </c>
       <c r="F6" t="n">
-        <v>0.331</v>
+        <v>0.361</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3</v>
+        <v>0.62</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>
@@ -669,66 +693,66 @@
       <c r="J6" t="n">
         <v>0</v>
       </c>
-      <c r="K6" t="s">
-        <v>15</v>
+      <c r="K6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E7" t="n">
-        <v>0.012</v>
+        <v>0.778</v>
       </c>
       <c r="F7" t="n">
-        <v>0.04</v>
+        <v>0.772</v>
       </c>
       <c r="G7" t="n">
-        <v>0.13</v>
+        <v>0.62</v>
       </c>
       <c r="H7" t="n">
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
       </c>
-      <c r="K7" t="s">
-        <v>15</v>
+      <c r="K7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.074</v>
       </c>
       <c r="F8" t="n">
-        <v>0.036</v>
+        <v>0.013</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1</v>
+        <v>0.47</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
@@ -739,171 +763,171 @@
       <c r="J8" t="n">
         <v>0</v>
       </c>
-      <c r="K8" t="s">
-        <v>15</v>
+      <c r="K8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" t="n">
-        <v>0.019</v>
+        <v>0.204</v>
       </c>
       <c r="F9" t="n">
-        <v>0.071</v>
+        <v>0.013</v>
       </c>
       <c r="G9" t="n">
-        <v>0.17</v>
+        <v>0.36</v>
       </c>
       <c r="H9" t="n">
         <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
       </c>
-      <c r="K9" t="s">
-        <v>15</v>
+      <c r="K9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" t="n">
-        <v>0.015</v>
+        <v>0.598</v>
       </c>
       <c r="F10" t="n">
-        <v>0.042</v>
+        <v>0.281</v>
       </c>
       <c r="G10" t="n">
-        <v>0.14</v>
+        <v>0.25</v>
       </c>
       <c r="H10" t="n">
         <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
       </c>
-      <c r="K10" t="s">
-        <v>15</v>
+      <c r="K10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" t="n">
-        <v>0.004</v>
+        <v>0.033</v>
       </c>
       <c r="F11" t="n">
-        <v>0.026</v>
+        <v>0.006</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1</v>
+        <v>0.42</v>
       </c>
       <c r="H11" t="n">
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
-      <c r="K11" t="s">
-        <v>15</v>
+      <c r="K11" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
       <c r="E12" t="n">
-        <v>0.005</v>
+        <v>0.01</v>
       </c>
       <c r="F12" t="n">
-        <v>0.024</v>
+        <v>0.047</v>
       </c>
       <c r="G12" t="n">
-        <v>0.16</v>
+        <v>0.21</v>
       </c>
       <c r="H12" t="n">
         <v>1</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.01</v>
+        <v>0.01</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
       </c>
-      <c r="K12" t="s">
-        <v>15</v>
+      <c r="K12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E13" t="n">
-        <v>0.008</v>
+        <v>0.021</v>
       </c>
       <c r="F13" t="n">
-        <v>0.068</v>
+        <v>0.044</v>
       </c>
       <c r="G13" t="n">
-        <v>0.16</v>
+        <v>0.28</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
@@ -914,66 +938,66 @@
       <c r="J13" t="n">
         <v>0</v>
       </c>
-      <c r="K13" t="s">
-        <v>15</v>
+      <c r="K13" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E14" t="n">
-        <v>0.087</v>
+        <v>0.655</v>
       </c>
       <c r="F14" t="n">
-        <v>0.06</v>
+        <v>0.585</v>
       </c>
       <c r="G14" t="n">
-        <v>0.14</v>
+        <v>0.33</v>
       </c>
       <c r="H14" t="n">
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
       </c>
-      <c r="K14" t="s">
-        <v>15</v>
+      <c r="K14" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E15" t="n">
-        <v>0.003</v>
+        <v>0.719</v>
       </c>
       <c r="F15" t="n">
-        <v>0.049</v>
+        <v>0.479</v>
       </c>
       <c r="G15" t="n">
-        <v>0.12</v>
+        <v>0.38</v>
       </c>
       <c r="H15" t="n">
         <v>1</v>
@@ -984,31 +1008,31 @@
       <c r="J15" t="n">
         <v>0</v>
       </c>
-      <c r="K15" t="s">
-        <v>15</v>
+      <c r="K15" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E16" t="n">
-        <v>0.076</v>
+        <v>0.674</v>
       </c>
       <c r="F16" t="n">
-        <v>0.022</v>
+        <v>0.331</v>
       </c>
       <c r="G16" t="n">
-        <v>0.53</v>
+        <v>0.3</v>
       </c>
       <c r="H16" t="n">
         <v>1</v>
@@ -1019,66 +1043,66 @@
       <c r="J16" t="n">
         <v>0</v>
       </c>
-      <c r="K16" t="s">
-        <v>15</v>
+      <c r="K16" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E17" t="n">
-        <v>0.162</v>
+        <v>0.012</v>
       </c>
       <c r="F17" t="n">
-        <v>0.023</v>
+        <v>0.04</v>
       </c>
       <c r="G17" t="n">
-        <v>0.45</v>
+        <v>0.13</v>
       </c>
       <c r="H17" t="n">
         <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="J17" t="n">
         <v>0</v>
       </c>
-      <c r="K17" t="s">
-        <v>15</v>
+      <c r="K17" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E18" t="n">
-        <v>0.743</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.605</v>
+        <v>0.036</v>
       </c>
       <c r="G18" t="n">
-        <v>0.18</v>
+        <v>0.1</v>
       </c>
       <c r="H18" t="n">
         <v>1</v>
@@ -1089,276 +1113,276 @@
       <c r="J18" t="n">
         <v>0</v>
       </c>
-      <c r="K18" t="s">
-        <v>15</v>
+      <c r="K18" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E19" t="n">
-        <v>0.204</v>
+        <v>0.019</v>
       </c>
       <c r="F19" t="n">
-        <v>0.199</v>
+        <v>0.071</v>
       </c>
       <c r="G19" t="n">
-        <v>0.22</v>
+        <v>0.17</v>
       </c>
       <c r="H19" t="n">
         <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
       </c>
-      <c r="K19" t="s">
-        <v>15</v>
+      <c r="K19" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
         <v>34</v>
       </c>
       <c r="E20" t="n">
-        <v>0.606</v>
+        <v>0.015</v>
       </c>
       <c r="F20" t="n">
-        <v>0.614</v>
+        <v>0.042</v>
       </c>
       <c r="G20" t="n">
-        <v>0.45</v>
+        <v>0.14</v>
       </c>
       <c r="H20" t="n">
         <v>1</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="J20" t="n">
         <v>0</v>
       </c>
-      <c r="K20" t="s">
-        <v>15</v>
+      <c r="K20" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
         <v>35</v>
       </c>
       <c r="E21" t="n">
-        <v>0.126</v>
+        <v>0.004</v>
       </c>
       <c r="F21" t="n">
-        <v>0.015</v>
+        <v>0.026</v>
       </c>
       <c r="G21" t="n">
-        <v>0.39</v>
+        <v>0.1</v>
       </c>
       <c r="H21" t="n">
         <v>1</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
       </c>
-      <c r="K21" t="s">
-        <v>15</v>
+      <c r="K21" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E22" t="n">
-        <v>0.774</v>
+        <v>0.005</v>
       </c>
       <c r="F22" t="n">
-        <v>0.647</v>
+        <v>0.024</v>
       </c>
       <c r="G22" t="n">
-        <v>0.47</v>
+        <v>0.16</v>
       </c>
       <c r="H22" t="n">
         <v>1</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
       </c>
-      <c r="K22" t="s">
-        <v>15</v>
+      <c r="K22" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E23" t="n">
-        <v>0.172</v>
+        <v>0.008</v>
       </c>
       <c r="F23" t="n">
-        <v>0.042</v>
+        <v>0.068</v>
       </c>
       <c r="G23" t="n">
-        <v>0.49</v>
+        <v>0.16</v>
       </c>
       <c r="H23" t="n">
         <v>1</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="J23" t="n">
         <v>0</v>
       </c>
-      <c r="K23" t="s">
-        <v>15</v>
+      <c r="K23" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
         <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E24" t="n">
-        <v>0.078</v>
+        <v>0.087</v>
       </c>
       <c r="F24" t="n">
-        <v>0.014</v>
+        <v>0.06</v>
       </c>
       <c r="G24" t="n">
-        <v>0.37</v>
+        <v>0.14</v>
       </c>
       <c r="H24" t="n">
         <v>1</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="J24" t="n">
         <v>0</v>
       </c>
-      <c r="K24" t="s">
-        <v>15</v>
+      <c r="K24" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
         <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E25" t="n">
-        <v>0.304</v>
+        <v>0.003</v>
       </c>
       <c r="F25" t="n">
-        <v>0.486</v>
+        <v>0.049</v>
       </c>
       <c r="G25" t="n">
-        <v>0.32</v>
+        <v>0.12</v>
       </c>
       <c r="H25" t="n">
         <v>1</v>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="J25" t="n">
         <v>0</v>
       </c>
-      <c r="K25" t="s">
-        <v>15</v>
+      <c r="K25" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E26" t="n">
-        <v>0.2</v>
+        <v>0.076</v>
       </c>
       <c r="F26" t="n">
-        <v>0.012</v>
+        <v>0.022</v>
       </c>
       <c r="G26" t="n">
-        <v>0.31</v>
+        <v>0.53</v>
       </c>
       <c r="H26" t="n">
         <v>1</v>
@@ -1369,31 +1393,31 @@
       <c r="J26" t="n">
         <v>0</v>
       </c>
-      <c r="K26" t="s">
-        <v>15</v>
+      <c r="K26" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E27" t="n">
-        <v>0.167</v>
+        <v>0.162</v>
       </c>
       <c r="F27" t="n">
         <v>0.023</v>
       </c>
       <c r="G27" t="n">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="H27" t="n">
         <v>1</v>
@@ -1404,31 +1428,31 @@
       <c r="J27" t="n">
         <v>0</v>
       </c>
-      <c r="K27" t="s">
-        <v>15</v>
+      <c r="K27" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
         <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E28" t="n">
-        <v>0.826</v>
+        <v>0.743</v>
       </c>
       <c r="F28" t="n">
-        <v>0.583</v>
+        <v>0.605</v>
       </c>
       <c r="G28" t="n">
-        <v>0.58</v>
+        <v>0.18</v>
       </c>
       <c r="H28" t="n">
         <v>1</v>
@@ -1439,31 +1463,31 @@
       <c r="J28" t="n">
         <v>0</v>
       </c>
-      <c r="K28" t="s">
-        <v>15</v>
+      <c r="K28" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
         <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E29" t="n">
-        <v>0.72</v>
+        <v>0.204</v>
       </c>
       <c r="F29" t="n">
-        <v>0.52</v>
+        <v>0.199</v>
       </c>
       <c r="G29" t="n">
-        <v>0.52</v>
+        <v>0.22</v>
       </c>
       <c r="H29" t="n">
         <v>1</v>
@@ -1474,31 +1498,31 @@
       <c r="J29" t="n">
         <v>0</v>
       </c>
-      <c r="K29" t="s">
-        <v>15</v>
+      <c r="K29" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
         <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E30" t="n">
-        <v>0.375</v>
+        <v>0.606</v>
       </c>
       <c r="F30" t="n">
-        <v>0.018</v>
+        <v>0.614</v>
       </c>
       <c r="G30" t="n">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="H30" t="n">
         <v>1</v>
@@ -1509,31 +1533,31 @@
       <c r="J30" t="n">
         <v>0</v>
       </c>
-      <c r="K30" t="s">
-        <v>15</v>
+      <c r="K30" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
         <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E31" t="n">
-        <v>0.102</v>
+        <v>0.126</v>
       </c>
       <c r="F31" t="n">
-        <v>0.008</v>
+        <v>0.015</v>
       </c>
       <c r="G31" t="n">
-        <v>0.36</v>
+        <v>0.39</v>
       </c>
       <c r="H31" t="n">
         <v>1</v>
@@ -1544,31 +1568,31 @@
       <c r="J31" t="n">
         <v>0</v>
       </c>
-      <c r="K31" t="s">
-        <v>15</v>
+      <c r="K31" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D32" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E32" t="n">
-        <v>0.212</v>
+        <v>0.774</v>
       </c>
       <c r="F32" t="n">
-        <v>0.117</v>
+        <v>0.647</v>
       </c>
       <c r="G32" t="n">
-        <v>0.28</v>
+        <v>0.47</v>
       </c>
       <c r="H32" t="n">
         <v>1</v>
@@ -1579,31 +1603,31 @@
       <c r="J32" t="n">
         <v>0</v>
       </c>
-      <c r="K32" t="s">
-        <v>15</v>
+      <c r="K32" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E33" t="n">
-        <v>0.051</v>
+        <v>0.172</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="G33" t="n">
-        <v>0.07</v>
+        <v>0.49</v>
       </c>
       <c r="H33" t="n">
         <v>1</v>
@@ -1614,31 +1638,31 @@
       <c r="J33" t="n">
         <v>0</v>
       </c>
-      <c r="K33" t="s">
-        <v>15</v>
+      <c r="K33" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C34" t="s">
         <v>13</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="E34" t="n">
-        <v>0.618</v>
+        <v>0.078</v>
       </c>
       <c r="F34" t="n">
-        <v>0.472</v>
+        <v>0.014</v>
       </c>
       <c r="G34" t="n">
-        <v>0.35</v>
+        <v>0.37</v>
       </c>
       <c r="H34" t="n">
         <v>1</v>
@@ -1649,31 +1673,31 @@
       <c r="J34" t="n">
         <v>0</v>
       </c>
-      <c r="K34" t="s">
-        <v>15</v>
+      <c r="K34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C35" t="s">
         <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="E35" t="n">
-        <v>0.04</v>
+        <v>0.304</v>
       </c>
       <c r="F35" t="n">
-        <v>0.191</v>
+        <v>0.486</v>
       </c>
       <c r="G35" t="n">
-        <v>0.36</v>
+        <v>0.32</v>
       </c>
       <c r="H35" t="n">
         <v>1</v>
@@ -1684,31 +1708,31 @@
       <c r="J35" t="n">
         <v>0</v>
       </c>
-      <c r="K35" t="s">
-        <v>15</v>
+      <c r="K35" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
         <v>13</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="E36" t="n">
-        <v>0.713</v>
+        <v>0.2</v>
       </c>
       <c r="F36" t="n">
-        <v>0.325</v>
+        <v>0.012</v>
       </c>
       <c r="G36" t="n">
-        <v>0.28</v>
+        <v>0.31</v>
       </c>
       <c r="H36" t="n">
         <v>1</v>
@@ -1719,31 +1743,31 @@
       <c r="J36" t="n">
         <v>0</v>
       </c>
-      <c r="K36" t="s">
-        <v>15</v>
+      <c r="K36" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C37" t="s">
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E37" t="n">
-        <v>0.766</v>
+        <v>0.167</v>
       </c>
       <c r="F37" t="n">
-        <v>0.779</v>
+        <v>0.023</v>
       </c>
       <c r="G37" t="n">
-        <v>0.43</v>
+        <v>0.3</v>
       </c>
       <c r="H37" t="n">
         <v>1</v>
@@ -1754,31 +1778,31 @@
       <c r="J37" t="n">
         <v>0</v>
       </c>
-      <c r="K37" t="s">
-        <v>15</v>
+      <c r="K37" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
         <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="E38" t="n">
-        <v>0.012</v>
+        <v>0.826</v>
       </c>
       <c r="F38" t="n">
-        <v>0.071</v>
+        <v>0.583</v>
       </c>
       <c r="G38" t="n">
-        <v>0.22</v>
+        <v>0.58</v>
       </c>
       <c r="H38" t="n">
         <v>1</v>
@@ -1789,31 +1813,31 @@
       <c r="J38" t="n">
         <v>0</v>
       </c>
-      <c r="K38" t="s">
-        <v>15</v>
+      <c r="K38" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
         <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="E39" t="n">
-        <v>0.028</v>
+        <v>0.72</v>
       </c>
       <c r="F39" t="n">
-        <v>0.161</v>
+        <v>0.52</v>
       </c>
       <c r="G39" t="n">
-        <v>0.08</v>
+        <v>0.52</v>
       </c>
       <c r="H39" t="n">
         <v>1</v>
@@ -1824,66 +1848,66 @@
       <c r="J39" t="n">
         <v>0</v>
       </c>
-      <c r="K39" t="s">
-        <v>15</v>
+      <c r="K39" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
         <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E40" t="n">
-        <v>0.045</v>
+        <v>0.375</v>
       </c>
       <c r="F40" t="n">
-        <v>0.052</v>
+        <v>0.018</v>
       </c>
       <c r="G40" t="n">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="H40" t="n">
         <v>1</v>
       </c>
       <c r="I40" t="n">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="J40" t="n">
         <v>0</v>
       </c>
-      <c r="K40" t="s">
-        <v>15</v>
+      <c r="K40" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C41" t="s">
         <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E41" t="n">
-        <v>0.026</v>
+        <v>0.102</v>
       </c>
       <c r="F41" t="n">
-        <v>0.046</v>
+        <v>0.008</v>
       </c>
       <c r="G41" t="n">
-        <v>0.18</v>
+        <v>0.36</v>
       </c>
       <c r="H41" t="n">
         <v>1</v>
@@ -1894,43 +1918,393 @@
       <c r="J41" t="n">
         <v>0</v>
       </c>
-      <c r="K41" t="s">
-        <v>15</v>
+      <c r="K41" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
         <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E42" t="n">
+        <v>0.212</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.117</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="H43" t="n">
+        <v>1</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.618</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.472</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.191</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" t="s">
+        <v>29</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.713</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.325</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="H46" t="n">
+        <v>1</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.766</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.779</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="H47" t="n">
+        <v>1</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.071</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="H48" t="n">
+        <v>1</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.161</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="H49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H50" t="n">
+        <v>1</v>
+      </c>
+      <c r="I50" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="H51" t="n">
+        <v>1</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" t="n">
         <v>0.007</v>
       </c>
-      <c r="F42" t="n">
+      <c r="F52" t="n">
         <v>0.066</v>
       </c>
-      <c r="G42" t="n">
+      <c r="G52" t="n">
         <v>0.14</v>
       </c>
-      <c r="H42" t="n">
-        <v>1</v>
-      </c>
-      <c r="I42" t="n">
+      <c r="H52" t="n">
+        <v>1</v>
+      </c>
+      <c r="I52" t="n">
         <v>-0.01</v>
       </c>
-      <c r="J42" t="n">
-        <v>0</v>
-      </c>
-      <c r="K42" t="s">
-        <v>15</v>
+      <c r="J52" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>